<commit_message>
Prototype StageSelect/Perkins Floor Map Code.
</commit_message>
<xml_diff>
--- a/_planning/TILE_TYPES.xlsx
+++ b/_planning/TILE_TYPES.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="135" windowWidth="10455" windowHeight="6150"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Passable</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Sidewalk</t>
   </si>
   <si>
-    <t>Perkins Wall</t>
-  </si>
-  <si>
     <t>Dirt</t>
   </si>
   <si>
@@ -70,6 +67,15 @@
   </si>
   <si>
     <t>Perkins Stairs</t>
+  </si>
+  <si>
+    <t>Perkins Ceiling</t>
+  </si>
+  <si>
+    <t>Perkins Brick Wall</t>
+  </si>
+  <si>
+    <t>Perkins Tile Wall</t>
   </si>
 </sst>
 </file>
@@ -404,7 +410,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -447,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -456,7 +462,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -468,7 +474,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -480,9 +486,9 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -492,10 +498,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -504,7 +507,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -516,10 +519,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -528,16 +531,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -546,16 +543,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -564,10 +555,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -575,11 +572,29 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6">

</xml_diff>